<commit_message>
file cleanup, move old stuff to archive
</commit_message>
<xml_diff>
--- a/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
+++ b/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/CDIF/integrationPublic/XrayAbsorbtion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="395" documentId="8_{63F0368F-E27C-4D36-A8DB-1B09C9287864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A155E7-58B2-4935-BCFD-A6D996BDFB3B}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="8_{63F0368F-E27C-4D36-A8DB-1B09C9287864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B20D545D-94F0-4D66-A428-8F8C0607FAFD}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="390" windowWidth="28620" windowHeight="13875" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25965" windowHeight="14010" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="CDIF xas implementation" sheetId="1" r:id="rId1"/>
@@ -1085,13 +1085,13 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
@@ -1299,7 +1299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>74</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
fixing class and property names to align, update handling of x-ray detectors
</commit_message>
<xml_diff>
--- a/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
+++ b/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/CDIF/integrationPublic/XrayAbsorbtion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{63F0368F-E27C-4D36-A8DB-1B09C9287864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B20D545D-94F0-4D66-A428-8F8C0607FAFD}"/>
+  <xr:revisionPtr revIDLastSave="481" documentId="8_{63F0368F-E27C-4D36-A8DB-1B09C9287864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77EDDF83-60C8-4602-805C-D2EFFE471891}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25965" windowHeight="14010" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
+    <workbookView xWindow="975" yWindow="1140" windowWidth="27525" windowHeight="14010" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="CDIF xas implementation" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CDIF xas implementation'!$A$1:$E$61</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,6 +42,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stephen Richard</author>
+    <author>tc={9943886B-5F8D-4565-907E-C1FEF99CD84C}</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{39C5FCB3-EA31-48CA-A867-0CB051EE42EB}">
@@ -65,12 +69,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A47" authorId="1" shapeId="0" xr:uid="{9943886B-5F8D-4565-907E-C1FEF99CD84C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The specific detector used to measure a particular variable needs to be a property of the cdi:InstanceVariable/measurementTechnique</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="205">
   <si>
     <t>XAS field</t>
   </si>
@@ -455,70 +467,15 @@
     <t>either in schema:contributor[@type: 'schema:Role', schema:roleName: 'Facility', OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalProperty, propertyID = nxs:Field/NXsource/type</t>
   </si>
   <si>
-    <t>prov:wasGeneratedBy/nxs:instrument[@type = thing]/additionalType = 'xas:Beamline'</t>
-  </si>
-  <si>
-    <t>either in schema:contributor[@type: 'schema:Role', schema:roleName: Facility, OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalPrpoerty, propertyID = xas:current</t>
-  </si>
-  <si>
-    <t>schema:additionalProperty : { schema:propertyID: xas:calculated,
-                                schema:value: true or false    },</t>
-  </si>
-  <si>
-    <t>xas:calculated in property vocabulary</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:collimation',          schema:value: text },</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:focusing',           schema:value: text },</t>
-  </si>
-  <si>
-    <t>xas:focusing in property vocabulary</t>
-  </si>
-  <si>
     <t>xas:harmonic_rejection in property vocabulary</t>
   </si>
   <si>
-    <t>prov:wasGeneratedBy/schema:mainEntity,
-                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:samplePreparation',</t>
-  </si>
-  <si>
-    <t>xas:samplePreparation in property vocabulary</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/schema:mainEntity,
-                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:parentSample',</t>
-  </si>
-  <si>
-    <t>xas:parentSample in property vocabulary</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/schema:mainEntity,
-                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:materialState',</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.i0',</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.it',</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.if',</t>
-  </si>
-  <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.ir',</t>
-  </si>
-  <si>
     <t>target edge for spectral analysis. Need vocabulary of absorption edges as defined in XDI spec, at least with a vocab URI to scope the defined terms, e.g. https://xas.org/vocab/absorptionedge.  Need xas:edge_energy</t>
   </si>
   <si>
     <t>need a vocab of elements, e.g. chebi or SWEET  http://sweetontology.net/matrElement for schema:inDefinedTermSet. Need xas:element</t>
   </si>
   <si>
-    <t>prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:harmonic_rejection',          schema:value: text },</t>
-  </si>
-  <si>
     <t>optional</t>
   </si>
   <si>
@@ -529,9 +486,6 @@
   </si>
   <si>
     <t>(profile = NXxas)(profile=NXxas_new) [nxs:Field/NXentry/definition]  or for XDI dc:conformstTo:["https://github.com/XraySpectroscopy/XAS-Data-Interchange/blob/master/specification/spec.md"]</t>
-  </si>
-  <si>
-    <t>default is false, element is optional.</t>
   </si>
   <si>
     <t>need xas:AnalysisEvent ,  multiple @types, also schema:Event and schema:Product.</t>
@@ -564,9 +518,6 @@
     <t>schema:measurementTechnique [schema:DefinedTerm]/schema:name, identifier; definedTermSet:nxs:Field/NXxas/ENTRY/DATA/mode</t>
   </si>
   <si>
-    <t>descriptions of how fluxes were measured; from XDI</t>
-  </si>
-  <si>
     <t>prov:wasGeneratedBy/schema:mainEntity,
                     schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'nxs:Field/NXsample/point_group',</t>
   </si>
@@ -581,9 +532,6 @@
                      additionalProperty:{ schema:propertyID: 'nxs:Field/NXsample/temperature',</t>
   </si>
   <si>
-    <t>prov:wasGeneratedBy/@type:Event, prov:Activity, 'xas:AnalysisEvent'</t>
-  </si>
-  <si>
     <t>is there other calibration besides detector?</t>
   </si>
   <si>
@@ -596,9 +544,6 @@
     <t>schema:contributor[@type: 'schema:Role'], schema:roleName: Facility,  "schema:contributor": {@type: schema:Organization, schema:name</t>
   </si>
   <si>
-    <t>either in schema:contributor[@type: 'schema:Role', schema:roleName: Facility, OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalProperty, propertyID = xas:energy</t>
-  </si>
-  <si>
     <t>nxs:Field/NXsource/energy</t>
   </si>
   <si>
@@ -617,9 +562,6 @@
     <t>various environmental parameters for sample analysis. These are extrinsic conditions imposed by the expermiental configuration, not intrinsic properties of the analyzed sample.</t>
   </si>
   <si>
-    <t>prov:wasGeneratedBy/@type:Event, additionalType='xas:AnalysisEvent',  prov:used[@type = Thing], additionalType = 'nxs:BaseClass/NXinstrument'</t>
-  </si>
-  <si>
     <t>prov:wasGeneratedBy/prov:used[@type = Thing], additionalType = 'nxs:BaseClass/NXinstrument'/ schema:name</t>
   </si>
   <si>
@@ -641,26 +583,149 @@
     <t>NXcollimator/type is limited to {"Soller" , "radial" , "oscillating" , "honeycomb"}</t>
   </si>
   <si>
-    <t>add xas:Beamline in vocabulary.  How is XDI beamline related to NEXUS NXbeam?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> nxs:Field/NXdetector/type</t>
   </si>
   <si>
-    <t>not sure about these….'how the incident flux was measured' from xdi.  NEXUS detector type examples: He3 gas cylinder, He3 PSD, scintillator, fission chamber, proportion counter, ion chamber, ccd, pixel, image plate, CMOS</t>
-  </si>
-  <si>
     <t>NEXUS note-- use space group if that is known.</t>
   </si>
   <si>
-    <t>xas:materialState in property vocabulary. Suggest using material type vocabulary like https://vocabs.ardc.edu.au/viewById/664</t>
+    <t>XAS skos uri</t>
+  </si>
+  <si>
+    <t>xas:calculated</t>
+  </si>
+  <si>
+    <t>xas:installedOptions</t>
+  </si>
+  <si>
+    <t>xas:Beamline</t>
+  </si>
+  <si>
+    <t>xas:collimation</t>
+  </si>
+  <si>
+    <t>xas:focusing</t>
+  </si>
+  <si>
+    <t>xas:harmonic_rejection</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/schema:mainEntity,
+                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:sample_material',</t>
+  </si>
+  <si>
+    <t>xas:sample_material</t>
+  </si>
+  <si>
+    <t>Instrument/detector/</t>
+  </si>
+  <si>
+    <t>xas:detector_type</t>
+  </si>
+  <si>
+    <t>in the instrument section, list the various detectors used to measure incident and transmitted or fluorescent intensity/flux</t>
+  </si>
+  <si>
+    <t>if different detectors are used for different variables, specify using an @id link from InstanceVariable to appropriate  instrument/detector instance. The same kind of detector might be used for different intensity measures.</t>
+  </si>
+  <si>
+    <t>schema:variableMeasured/@type=InstanceVariable/{..."schema:propertyID": {"@id": "xas:Transmitted_Intensity"},schema:measurementTechnique:{"@id":"uri for detector type instance"}</t>
+  </si>
+  <si>
+    <t>schema:variableMeasured/@type=InstanceVariable/{..."schema:propertyID": {"@id": "xas:Fluorescence_Intensity"},schema:measurementTechnique:{"@id":"uri for detector type instance"}</t>
+  </si>
+  <si>
+    <t>schema:variableMeasured/@type=InstanceVariable/{..."schema:propertyID": {"@id": "xas:Reference_Intensity"},schema:measurementTechnique:{"@id":"uri for detector type instance"}</t>
+  </si>
+  <si>
+    <t>xas:Reference_Intensity</t>
+  </si>
+  <si>
+    <t>xas:facility_energy</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalProperty, propertyID = xas:facility_energy</t>
+  </si>
+  <si>
+    <t>default is false, element is optional.  Is the property value derived by calculations after the measurement event.</t>
+  </si>
+  <si>
+    <t>xas:facility_current</t>
+  </si>
+  <si>
+    <t>Units should be A, mA, microA</t>
+  </si>
+  <si>
+    <t>units should be joules, product of current and particle energy.</t>
+  </si>
+  <si>
+    <t>either in schema:contributor[@type: 'schema:Role', schema:roleName: Facility, OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalPrpoerty, propertyID = xas:facility_current</t>
+  </si>
+  <si>
+    <t>schema:additionalProperty : { schema:propertyID: xas:calculated,  schema:value: true or false    },</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:Event, prov:Activity, 'xas:Analysis_Event'</t>
+  </si>
+  <si>
+    <t>xas:Analysis_Event</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event'],  prov:used[@type = Thing, prov:Entity, 'xas:Beamline']</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event'],  prov:used[@type = Thing, prov:Entity, 'xas:Beamline'], additionalProperty:{ schema:propertyID: 'xas:collimation',          schema:value: text },</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event'],  prov:used[@type = Thing, prov:Entity, 'xas:Beamline'], additionalProperty: { schema:propertyID: 'xas:harmonic_rejection', schema:value: text },</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event'],  prov:used[@type = Thing, prov:Entity, 'xas:Beamline'], additionalProperty: { schema:propertyID: 'xas:focusing',schema:value: text },</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event],  prov:used[@type = Thing, prov:Entity, nxs:Field/NXdetector'], additionalProperty: { schema:propertyID: 'xas:detector_type',</t>
+  </si>
+  <si>
+    <t>schema:variableMeasured/@type=InstanceVariable/ {..."schema:propertyID": {"@id": "xas:Incident_Intensity"}, schema:measurementTechnique: {"@id": "uri for detector type instance"}</t>
+  </si>
+  <si>
+    <t>xas:Instrument</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/@type:[Event,xas:Analysis_Event'],  prov:used[@type = Thing, prov:Entity, xas:Instrument], additionalType = 'nxs:BaseClass/NXinstrument'</t>
+  </si>
+  <si>
+    <t>partOf xas:Instrument, IsA xas:Instrument.  How is XDI beamline related to NEXUS NXbeam?</t>
+  </si>
+  <si>
+    <t>A statement about how beam focusing is provided</t>
+  </si>
+  <si>
+    <t>if different detectors are used for different variables, link variable to detector using an @id link from InstanceVariable to appropriate  instrument/detector instance. The same kind of detector might be used for different intensity measures.</t>
+  </si>
+  <si>
+    <t>xas:sample_preparation</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/schema:mainEntity,
+                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:sample_preparation',</t>
+  </si>
+  <si>
+    <t>xas:parent_sample</t>
+  </si>
+  <si>
+    <t>prov:wasGeneratedBy/schema:mainEntity,
+                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:parent_sample',</t>
+  </si>
+  <si>
+    <t>Suggest using material type vocabulary like https://vocabs.ardc.edu.au/viewById/664</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,6 +774,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -718,7 +789,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -726,11 +797,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -742,6 +893,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -762,7 +940,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Stephen Richard" id="{48BF9C19-F17B-4562-9DC2-4F4F51D80DE0}" userId="944a82e2ddcde9eb" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1080,13 +1260,22 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A47" dT="2025-09-27T19:28:10.01" personId="{48BF9C19-F17B-4562-9DC2-4F4F51D80DE0}" id="{9943886B-5F8D-4565-907E-C1FEF99CD84C}">
+    <text>The specific detector used to measure a particular variable needs to be a property of the cdi:InstanceVariable/measurementTechnique</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082CBB92-8BE8-4945-BD21-3498BF1AC68A}">
-  <dimension ref="A1:E60"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,10 +1285,11 @@
     <col min="3" max="3" width="51.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1115,8 +1305,11 @@
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1130,10 +1323,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1147,10 +1340,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
@@ -1164,128 +1357,144 @@
         <v>92</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="E5" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="E8" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1296,10 +1505,10 @@
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1307,33 +1516,33 @@
         <v>115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1344,10 +1553,10 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1358,18 +1567,23 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1377,16 +1591,16 @@
         <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1394,58 +1608,65 @@
         <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1453,13 +1674,13 @@
         <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1467,10 +1688,10 @@
         <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1481,10 +1702,10 @@
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1495,10 +1716,10 @@
         <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1509,10 +1730,10 @@
         <v>41</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1523,7 +1744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1534,7 +1755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1769,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1562,7 +1783,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1576,7 +1797,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -1590,18 +1811,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -1612,7 +1836,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>56</v>
       </c>
@@ -1620,16 +1844,19 @@
         <v>94</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>190</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -1637,13 +1864,16 @@
         <v>94</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1651,13 +1881,16 @@
         <v>94</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>142</v>
+        <v>191</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -1668,7 +1901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
@@ -1682,10 +1915,10 @@
         <v>69</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1699,209 +1932,244 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>186</v>
+      <c r="C61" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E61" xr:uid="{082CBB92-8BE8-4945-BD21-3498BF1AC68A}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="either in schema:contributor[@type: 'schema:Role', schema:roleName: Facility, OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalProperty, propertyID = xas:energy"/>
+        <filter val="either in schema:contributor[@type: 'schema:Role', schema:roleName: Facility, OR prov:wasGeneratedBy/@type:Event/schema:location,@type=Place…. additionalPrpoerty, propertyID = xas:current"/>
+        <filter val="prov:wasGeneratedBy/@type:Event, additionalType='xas:AnalysisEvent',  prov:used[@type = Thing], additionalType = 'nxs:BaseClass/NXinstrument'"/>
+        <filter val="prov:wasGeneratedBy/@type:Event, prov:Activity, 'xas:AnalysisEvent'"/>
+        <filter val="prov:wasGeneratedBy/additionalProperty:{ schema:propertyID: xas:installedOptions,_x000a_                                schema:value: text description or link    },"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.i0',"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.if',"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.ir',"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:BaseClass/NXdetector', additionalProperty:{ schema:propertyID: 'xas:detector.it',"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:collimation',          schema:value: text },"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:focusing',           schema:value: text },"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument/additionalType = 'nxs:beamline', additionalProperty:{ schema:propertyID: 'xas:harmonic_rejection',          schema:value: text },"/>
+        <filter val="prov:wasGeneratedBy/nxs:instrument[@type = thing]/additionalType = 'xas:Beamline'"/>
+        <filter val="prov:wasGeneratedBy/schema:mainEntity,_x000a_                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:materialState',"/>
+        <filter val="prov:wasGeneratedBy/schema:mainEntity,_x000a_                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:parentSample',"/>
+        <filter val="prov:wasGeneratedBy/schema:mainEntity,_x000a_                    schema:additionalType: MaterialSample, additionalProperty:{ schema:propertyID: 'xas:samplePreparation',"/>
+        <filter val="schema:additionalProperty : { schema:propertyID: xas:calculated,_x000a_                                schema:value: true or false    },"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
making sure latest changes are pushed
</commit_message>
<xml_diff>
--- a/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
+++ b/XrayAbsorbtion/XAS-CDIFImplementation.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="481" documentId="8_{63F0368F-E27C-4D36-A8DB-1B09C9287864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77EDDF83-60C8-4602-805C-D2EFFE471891}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1140" windowWidth="27525" windowHeight="14010" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7335" xr2:uid="{2A6E3241-1CD0-46EB-AFD7-A45E47D0E7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="CDIF xas implementation" sheetId="1" r:id="rId1"/>
@@ -725,7 +725,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,12 +773,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -881,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -905,9 +899,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1278,18 +1269,18 @@
       <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="28.265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.73046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.86328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1326,7 +1317,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1334,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
@@ -1360,7 +1351,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
@@ -1377,39 +1368,39 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:6" ht="28.9" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>104</v>
       </c>
@@ -1424,77 +1415,77 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>183</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:6" ht="57.4" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="99.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1508,7 +1499,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1525,7 +1516,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>149</v>
       </c>
@@ -1542,7 +1533,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1556,7 +1547,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="85.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1570,9 +1561,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>134</v>
       </c>
@@ -1583,7 +1574,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1600,7 +1591,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1614,7 +1605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>135</v>
       </c>
@@ -1631,7 +1622,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>141</v>
       </c>
@@ -1648,8 +1639,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1657,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1680,7 +1671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1682,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1705,7 +1696,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1719,7 +1710,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1733,7 +1724,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1744,7 +1735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1755,7 +1746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -1769,7 +1760,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1783,7 +1774,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1797,7 +1788,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -1811,7 +1802,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>54</v>
       </c>
@@ -1825,7 +1816,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -1836,7 +1827,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>56</v>
       </c>
@@ -1856,7 +1847,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -1873,7 +1864,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1890,7 +1881,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -1901,7 +1892,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
@@ -1918,7 +1909,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1932,7 +1923,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>171</v>
       </c>
@@ -1949,7 +1940,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -1963,7 +1954,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -1977,7 +1968,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1991,7 +1982,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>67</v>
       </c>
@@ -2008,8 +1999,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="1:6" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
@@ -2020,7 +2011,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -2031,7 +2022,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>76</v>
       </c>
@@ -2042,7 +2033,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>77</v>
       </c>
@@ -2056,7 +2047,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -2070,7 +2061,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>85</v>
       </c>
@@ -2084,7 +2075,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>86</v>
       </c>
@@ -2101,7 +2092,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>117</v>
       </c>
@@ -2115,7 +2106,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>118</v>
       </c>
@@ -2129,7 +2120,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>119</v>
       </c>

</xml_diff>